<commit_message>
cramer model working through console
</commit_message>
<xml_diff>
--- a/materiales_db.xlsx
+++ b/materiales_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abelm\Programacion\AyP2\4_AyP2_MOD2_TP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB56810-000D-45C3-9574-F863B16244AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6CF520-F43F-4942-B9BE-B07DCB936982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,201 +489,221 @@
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>7700</v>
+      </c>
+      <c r="D2" s="3">
+        <v>195000000000</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>7700</v>
-      </c>
-      <c r="D3" s="3">
-        <v>195000000000</v>
+        <v>2700</v>
+      </c>
+      <c r="D3" s="4">
+        <v>71000000000</v>
       </c>
       <c r="E3" s="4">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="F3" s="2">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>2700</v>
-      </c>
-      <c r="D4" s="4">
-        <v>71000000000</v>
+        <v>8500</v>
+      </c>
+      <c r="D4" s="3">
+        <v>95000000000</v>
       </c>
       <c r="E4" s="4">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F4" s="2">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>8500</v>
+        <v>8915</v>
       </c>
       <c r="D5" s="3">
-        <v>95000000000</v>
+        <v>127000000000</v>
       </c>
       <c r="E5" s="4">
         <v>0.01</v>
       </c>
       <c r="F5" s="2">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
-        <v>8915</v>
+        <v>600</v>
       </c>
       <c r="D6" s="3">
-        <v>127000000000</v>
+        <v>8300000000</v>
       </c>
       <c r="E6" s="4">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="F6" s="2">
-        <v>0.34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>600</v>
-      </c>
-      <c r="D7" s="3">
-        <v>8300000000</v>
+        <v>7700</v>
+      </c>
+      <c r="D7" s="4">
+        <v>195000000000.00003</v>
       </c>
       <c r="E7" s="4">
-        <v>0.05</v>
+        <v>1E-4</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
-        <v>7700</v>
-      </c>
-      <c r="D8" s="4">
-        <v>195000000000.00003</v>
+        <v>2400</v>
+      </c>
+      <c r="D8" s="3">
+        <v>30000000000</v>
       </c>
       <c r="E8" s="4">
-        <v>1E-4</v>
+        <v>0.05</v>
       </c>
       <c r="F8" s="2">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>2400</v>
+        <v>900</v>
       </c>
       <c r="D9" s="3">
-        <v>30000000000</v>
+        <v>4800000000</v>
       </c>
       <c r="E9" s="4">
         <v>0.05</v>
       </c>
       <c r="F9" s="2">
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
-        <v>900</v>
-      </c>
-      <c r="D10" s="3">
-        <v>4800000000</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.05</v>
+        <v>2100</v>
+      </c>
+      <c r="D10" s="2">
+        <f>2.5*(10^10)</f>
+        <v>25000000000</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.01</v>
       </c>
       <c r="F10" s="2">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2">
-        <v>2100</v>
-      </c>
-      <c r="D11" s="2">
-        <f>2.5*(10^10)</f>
-        <v>25000000000</v>
-      </c>
-      <c r="E11" s="2">
+        <v>650</v>
+      </c>
+      <c r="D11" s="4">
+        <v>12000000000</v>
+      </c>
+      <c r="E11" s="5">
         <v>0.01</v>
       </c>
       <c r="F11" s="2">
@@ -692,101 +712,81 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
-        <v>650</v>
-      </c>
-      <c r="D12" s="4">
-        <v>12000000000</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.01</v>
+        <v>1200</v>
+      </c>
+      <c r="D12" s="3">
+        <v>100000000</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.1</v>
       </c>
       <c r="F12" s="2">
-        <v>0.15</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
-        <v>1200</v>
-      </c>
-      <c r="D13" s="3">
-        <v>100000000</v>
+        <v>11300</v>
+      </c>
+      <c r="D13" s="4">
+        <v>17000000000.000002</v>
       </c>
       <c r="E13" s="4">
-        <v>0.1</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="F13" s="2">
-        <v>0.49</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
-        <v>11300</v>
-      </c>
-      <c r="D14" s="4">
-        <v>17000000000.000002</v>
+        <v>2500</v>
+      </c>
+      <c r="D14" s="3">
+        <v>68000000000</v>
       </c>
       <c r="E14" s="4">
-        <v>5.0000000000000001E-4</v>
+        <v>0.02</v>
       </c>
       <c r="F14" s="2">
-        <v>0.15</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2">
-        <v>2500</v>
-      </c>
-      <c r="D15" s="3">
-        <v>68000000000</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0.02</v>
+        <v>800</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2000000000</v>
+      </c>
+      <c r="E15" s="3">
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F15" s="2">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="2">
-        <v>800</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2000000000</v>
-      </c>
-      <c r="E16" s="3">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="F16" s="2">
         <v>0.24</v>
       </c>
     </row>

</xml_diff>